<commit_message>
modify game variable ajustment
</commit_message>
<xml_diff>
--- a/Docs/score.xlsx
+++ b/Docs/score.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projets\Matematiks\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975DAAF5-99C6-414A-AE06-A66F8CC24DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57257B-6310-414C-B72D-7F4273CA8BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{74EC0562-3478-4967-B28E-D5CE58C0BC47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{74EC0562-3478-4967-B28E-D5CE58C0BC47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Score" sheetId="1" r:id="rId1"/>
+    <sheet name="Gem" sheetId="2" r:id="rId2"/>
+    <sheet name="WeightedBall" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
   <si>
     <t>actuel</t>
   </si>
@@ -89,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -107,6 +108,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2065,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D113C6E-381B-4269-A5E0-70BB64F2B0BE}">
   <dimension ref="B1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,4 +3700,1787 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BBAEDE-1245-4FD8-9D9E-C9EF3607900C}">
+  <dimension ref="A1:E105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="5" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <f>$A$2+$C$2/$B$2</f>
+        <v>6.5</v>
+      </c>
+      <c r="D4" s="7">
+        <f>B4/$B$2+$C$2/$B$2</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <f>B4/$B$2+$C$2</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ref="C5:C68" si="0">$A$2+$C$2/$B$2</f>
+        <v>6.5</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ref="D5:D68" si="1">B5/$B$2+$C$2/$B$2</f>
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E68" si="2">B5/$B$2+$C$2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="2"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="2"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>21</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="2"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>23</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="1"/>
+        <v>13.5</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>25</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>26</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="2"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>28</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="1"/>
+        <v>15.5</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>29</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="2"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>30</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>31</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="2"/>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>32</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>33</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="2"/>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>34</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="1"/>
+        <v>18.5</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>35</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="2"/>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>36</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>37</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="1"/>
+        <v>20.5</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>39</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="E42" s="7">
+        <f t="shared" si="2"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>40</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="1"/>
+        <v>21.5</v>
+      </c>
+      <c r="E43" s="7">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>41</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E44" s="7">
+        <f t="shared" si="2"/>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>42</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>43</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="2"/>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>44</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="1"/>
+        <v>23.5</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>45</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="2"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>46</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="1"/>
+        <v>24.5</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>47</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="2"/>
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>48</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>49</v>
+      </c>
+      <c r="C52" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="2"/>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>50</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="1"/>
+        <v>26.5</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>51</v>
+      </c>
+      <c r="C54" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="2"/>
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>52</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="1"/>
+        <v>27.5</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>53</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E56" s="7">
+        <f t="shared" si="2"/>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>54</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="1"/>
+        <v>28.5</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>55</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="E58" s="7">
+        <f t="shared" si="2"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>56</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="E59" s="7">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>57</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="2"/>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>58</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="1"/>
+        <v>30.5</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>59</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" si="2"/>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>60</v>
+      </c>
+      <c r="C63" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="1"/>
+        <v>31.5</v>
+      </c>
+      <c r="E63" s="7">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>61</v>
+      </c>
+      <c r="C64" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D64" s="7">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="E64" s="7">
+        <f t="shared" si="2"/>
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
+        <v>62</v>
+      </c>
+      <c r="C65" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D65" s="7">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
+      </c>
+      <c r="E65" s="7">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>63</v>
+      </c>
+      <c r="C66" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="E66" s="7">
+        <f t="shared" si="2"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>64</v>
+      </c>
+      <c r="C67" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D67" s="7">
+        <f t="shared" si="1"/>
+        <v>33.5</v>
+      </c>
+      <c r="E67" s="7">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>65</v>
+      </c>
+      <c r="C68" s="7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D68" s="7">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E68" s="7">
+        <f t="shared" si="2"/>
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>66</v>
+      </c>
+      <c r="C69" s="7">
+        <f t="shared" ref="C69:C105" si="3">$A$2+$C$2/$B$2</f>
+        <v>6.5</v>
+      </c>
+      <c r="D69" s="7">
+        <f t="shared" ref="D69:D103" si="4">B69/$B$2+$C$2/$B$2</f>
+        <v>34.5</v>
+      </c>
+      <c r="E69" s="7">
+        <f t="shared" ref="E69:E105" si="5">B69/$B$2+$C$2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>67</v>
+      </c>
+      <c r="C70" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D70" s="7">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="E70" s="7">
+        <f t="shared" si="5"/>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>68</v>
+      </c>
+      <c r="C71" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D71" s="7">
+        <f t="shared" si="4"/>
+        <v>35.5</v>
+      </c>
+      <c r="E71" s="7">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>69</v>
+      </c>
+      <c r="C72" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D72" s="7">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="E72" s="7">
+        <f t="shared" si="5"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
+        <v>70</v>
+      </c>
+      <c r="C73" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D73" s="7">
+        <f t="shared" si="4"/>
+        <v>36.5</v>
+      </c>
+      <c r="E73" s="7">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>71</v>
+      </c>
+      <c r="C74" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D74" s="7">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="E74" s="7">
+        <f t="shared" si="5"/>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
+        <v>72</v>
+      </c>
+      <c r="C75" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D75" s="7">
+        <f t="shared" si="4"/>
+        <v>37.5</v>
+      </c>
+      <c r="E75" s="7">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
+        <v>73</v>
+      </c>
+      <c r="C76" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D76" s="7">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="E76" s="7">
+        <f t="shared" si="5"/>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>74</v>
+      </c>
+      <c r="C77" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D77" s="7">
+        <f t="shared" si="4"/>
+        <v>38.5</v>
+      </c>
+      <c r="E77" s="7">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>75</v>
+      </c>
+      <c r="C78" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D78" s="7">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="E78" s="7">
+        <f t="shared" si="5"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
+        <v>76</v>
+      </c>
+      <c r="C79" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D79" s="7">
+        <f t="shared" si="4"/>
+        <v>39.5</v>
+      </c>
+      <c r="E79" s="7">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
+        <v>77</v>
+      </c>
+      <c r="C80" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D80" s="7">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="E80" s="7">
+        <f t="shared" si="5"/>
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
+        <v>78</v>
+      </c>
+      <c r="C81" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" si="4"/>
+        <v>40.5</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
+        <v>79</v>
+      </c>
+      <c r="C82" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="E82" s="7">
+        <f t="shared" si="5"/>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
+        <v>80</v>
+      </c>
+      <c r="C83" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D83" s="7">
+        <f t="shared" si="4"/>
+        <v>41.5</v>
+      </c>
+      <c r="E83" s="7">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1">
+        <v>81</v>
+      </c>
+      <c r="C84" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D84" s="7">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="E84" s="7">
+        <f t="shared" si="5"/>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="1">
+        <v>82</v>
+      </c>
+      <c r="C85" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D85" s="7">
+        <f t="shared" si="4"/>
+        <v>42.5</v>
+      </c>
+      <c r="E85" s="7">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="1">
+        <v>83</v>
+      </c>
+      <c r="C86" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D86" s="7">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="E86" s="7">
+        <f t="shared" si="5"/>
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="1">
+        <v>84</v>
+      </c>
+      <c r="C87" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" si="4"/>
+        <v>43.5</v>
+      </c>
+      <c r="E87" s="7">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
+        <v>85</v>
+      </c>
+      <c r="C88" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D88" s="7">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="E88" s="7">
+        <f t="shared" si="5"/>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="1">
+        <v>86</v>
+      </c>
+      <c r="C89" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D89" s="7">
+        <f t="shared" si="4"/>
+        <v>44.5</v>
+      </c>
+      <c r="E89" s="7">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="1">
+        <v>87</v>
+      </c>
+      <c r="C90" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D90" s="7">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="E90" s="7">
+        <f t="shared" si="5"/>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="1">
+        <v>88</v>
+      </c>
+      <c r="C91" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" si="4"/>
+        <v>45.5</v>
+      </c>
+      <c r="E91" s="7">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="1">
+        <v>89</v>
+      </c>
+      <c r="C92" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="E92" s="7">
+        <f t="shared" si="5"/>
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="1">
+        <v>90</v>
+      </c>
+      <c r="C93" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D93" s="7">
+        <f t="shared" si="4"/>
+        <v>46.5</v>
+      </c>
+      <c r="E93" s="7">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="1">
+        <v>91</v>
+      </c>
+      <c r="C94" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D94" s="7">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="E94" s="7">
+        <f t="shared" si="5"/>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="1">
+        <v>92</v>
+      </c>
+      <c r="C95" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D95" s="7">
+        <f t="shared" si="4"/>
+        <v>47.5</v>
+      </c>
+      <c r="E95" s="7">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
+        <v>93</v>
+      </c>
+      <c r="C96" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D96" s="7">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="E96" s="7">
+        <f t="shared" si="5"/>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
+        <v>94</v>
+      </c>
+      <c r="C97" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D97" s="7">
+        <f t="shared" si="4"/>
+        <v>48.5</v>
+      </c>
+      <c r="E97" s="7">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="1">
+        <v>95</v>
+      </c>
+      <c r="C98" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D98" s="7">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="E98" s="7">
+        <f t="shared" si="5"/>
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="1">
+        <v>96</v>
+      </c>
+      <c r="C99" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D99" s="7">
+        <f t="shared" si="4"/>
+        <v>49.5</v>
+      </c>
+      <c r="E99" s="7">
+        <f t="shared" si="5"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="1">
+        <v>97</v>
+      </c>
+      <c r="C100" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D100" s="7">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="E100" s="7">
+        <f t="shared" si="5"/>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="1">
+        <v>98</v>
+      </c>
+      <c r="C101" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D101" s="7">
+        <f t="shared" si="4"/>
+        <v>50.5</v>
+      </c>
+      <c r="E101" s="7">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
+        <v>99</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D102" s="7">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="E102" s="7">
+        <f t="shared" si="5"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="1">
+        <v>100</v>
+      </c>
+      <c r="C103" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D103" s="7">
+        <f t="shared" si="4"/>
+        <v>51.5</v>
+      </c>
+      <c r="E103" s="7">
+        <f t="shared" si="5"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="1">
+        <v>500</v>
+      </c>
+      <c r="C104" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D104" s="7">
+        <f t="shared" ref="D104" si="6">B104/$B$2+$C$2/$B$2</f>
+        <v>251.5</v>
+      </c>
+      <c r="E104" s="7">
+        <f t="shared" si="5"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C105" s="7">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D105" s="7">
+        <f t="shared" ref="D105" si="7">B105/$B$2+$C$2/$B$2</f>
+        <v>501.5</v>
+      </c>
+      <c r="E105" s="7">
+        <f t="shared" si="5"/>
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>